<commit_message>
Weapons (Gunshots & Blasters)
</commit_message>
<xml_diff>
--- a/Other/weaponsBalance.xlsx
+++ b/Other/weaponsBalance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danit\Desktop\Github\Unity_MultiplayerGame\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A913390-2190-4EB0-8967-CBC4A6DDF21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8539F462-2901-4C8C-91CB-00B11ED424B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8BFD530-F1DB-4083-B445-48265BEB5EB8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Wp</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Ink efficience</t>
-  </si>
-  <si>
     <t>RNG</t>
   </si>
   <si>
@@ -134,10 +131,31 @@
     <t>pps</t>
   </si>
   <si>
-    <t xml:space="preserve"> (10 dmg x 9 bullet)</t>
-  </si>
-  <si>
     <t>bullet speed</t>
+  </si>
+  <si>
+    <t>Bullets per shot</t>
+  </si>
+  <si>
+    <t>Pellets</t>
+  </si>
+  <si>
+    <t>Blasters</t>
+  </si>
+  <si>
+    <t>Shots per tank</t>
+  </si>
+  <si>
+    <t>indirect dmg</t>
+  </si>
+  <si>
+    <t>fallof or</t>
+  </si>
+  <si>
+    <t>70-35</t>
+  </si>
+  <si>
+    <t>35-25</t>
   </si>
 </sst>
 </file>
@@ -187,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +248,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -412,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -420,7 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -465,9 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,9 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -556,13 +585,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -570,6 +595,55 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +659,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -888,128 +958,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E3534C-2912-465D-8271-A50631F92518}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="19" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="6" t="s">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="L2" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="29" t="s">
+      <c r="O2" s="3"/>
+      <c r="Q2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="4"/>
-      <c r="Q2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="60">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2">
-        <v>36</v>
       </c>
       <c r="E4" s="2">
         <v>8</v>
@@ -1018,359 +1105,627 @@
         <f>1/E4</f>
         <v>0.125</v>
       </c>
-      <c r="G4" s="8">
-        <f>D4*E4</f>
+      <c r="G4" s="7">
+        <f>C4*E4*D4</f>
         <v>288</v>
       </c>
-      <c r="H4" s="16">
-        <f>100/D4</f>
+      <c r="H4" s="15">
+        <f t="shared" ref="H4:H13" si="0">100/C4</f>
         <v>2.7777777777777777</v>
       </c>
       <c r="I4" s="2">
         <v>0.8</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <f>100/I4</f>
         <v>125</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="44">
         <v>15</v>
       </c>
-      <c r="L4" s="48">
+      <c r="L4" s="45">
         <v>3</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="57">
         <v>0.75</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="18">
         <v>3</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="21">
         <v>3</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="19">
         <v>2</v>
       </c>
-      <c r="Q4" s="17">
-        <f>N4+O4*P4</f>
+      <c r="Q4" s="16">
+        <f>N4*D4+O4*P4*D4</f>
         <v>9</v>
       </c>
-      <c r="R4" s="17">
+      <c r="R4" s="62">
         <f>E4*Q4</f>
         <v>72</v>
       </c>
-      <c r="S4" s="54">
+      <c r="S4" s="49">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="C5" s="60">
         <v>28</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>10.3</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F9" si="0">1/E5</f>
+        <f t="shared" ref="F5:F13" si="1">1/E5</f>
         <v>9.7087378640776698E-2</v>
       </c>
-      <c r="G5" s="8">
-        <f t="shared" ref="G5:G9" si="1">D5*E5</f>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G13" si="2">C5*E5*D5</f>
         <v>288.40000000000003</v>
       </c>
-      <c r="H5" s="17">
-        <f t="shared" ref="H5:H9" si="2">100/D5</f>
+      <c r="H5" s="16">
+        <f t="shared" si="0"/>
         <v>3.5714285714285716</v>
       </c>
       <c r="I5" s="2">
         <v>0.71</v>
       </c>
-      <c r="J5" s="9">
-        <f t="shared" ref="J5:J9" si="3">100/I5</f>
+      <c r="J5" s="8">
+        <f t="shared" ref="J5:J13" si="3">100/I5</f>
         <v>140.84507042253523</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="46">
         <v>15</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>2.5</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5" s="58">
         <v>0.8</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="20">
         <v>3</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="21">
         <v>4</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="22">
         <v>2</v>
       </c>
-      <c r="Q5" s="17">
-        <f t="shared" ref="Q5:Q8" si="4">N5+O5*P5</f>
+      <c r="Q5" s="16">
+        <f t="shared" ref="Q5:Q8" si="4">N5*D5+O5*P5*D5</f>
         <v>11</v>
       </c>
-      <c r="R5" s="17">
+      <c r="R5" s="62">
         <f t="shared" ref="R5:R8" si="5">E5*Q5</f>
         <v>113.30000000000001</v>
       </c>
-      <c r="S5" s="42">
+      <c r="S5" s="40">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="C6" s="60">
         <v>52</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
       </c>
       <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="2"/>
+        <v>312</v>
+      </c>
+      <c r="H6" s="16">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G6" s="8">
-        <f t="shared" si="1"/>
-        <v>312</v>
-      </c>
-      <c r="H6" s="17">
-        <f t="shared" si="2"/>
         <v>1.9230769230769231</v>
       </c>
       <c r="I6" s="2">
         <v>1.65</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <f t="shared" si="3"/>
         <v>60.606060606060609</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="46">
         <v>18</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="12">
         <v>4.5</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="58">
         <v>0.5</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="20">
         <v>3.5</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="21">
         <v>2</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="22">
         <v>2.25</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="16">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="R6" s="17">
+      <c r="R6" s="62">
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="S6" s="42">
+      <c r="S6" s="40">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="11" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
+      <c r="C7" s="60">
         <v>42</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>7</v>
       </c>
       <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="2"/>
+        <v>294</v>
+      </c>
+      <c r="H7" s="16">
         <f t="shared" si="0"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="G7" s="8">
-        <f t="shared" si="1"/>
-        <v>294</v>
-      </c>
-      <c r="H7" s="17">
-        <f t="shared" si="2"/>
         <v>2.3809523809523809</v>
       </c>
       <c r="I7" s="2">
         <v>1.25</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="K7" s="49">
-        <v>30</v>
-      </c>
-      <c r="L7" s="13">
+      <c r="K7" s="46">
+        <v>28</v>
+      </c>
+      <c r="L7" s="12">
         <v>1.5</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="58">
         <v>0.65</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="20">
         <v>3.4</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="21">
         <v>3</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="22">
         <v>2</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="16">
         <f t="shared" si="4"/>
         <v>9.4</v>
       </c>
-      <c r="R7" s="17">
+      <c r="R7" s="62">
         <f t="shared" si="5"/>
         <v>65.8</v>
       </c>
-      <c r="S7" s="42">
+      <c r="S7" s="40">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="11" t="s">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="5">
+      <c r="C8" s="61">
         <v>33</v>
       </c>
-      <c r="E8" s="5">
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
         <v>15</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G8" s="52">
+        <f t="shared" si="2"/>
+        <v>495</v>
+      </c>
+      <c r="H8" s="17">
         <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="G8" s="46">
-        <f t="shared" si="1"/>
-        <v>495</v>
-      </c>
-      <c r="H8" s="18">
-        <f t="shared" si="2"/>
         <v>3.0303030303030303</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <f>0.45</f>
         <v>0.45</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <f t="shared" si="3"/>
         <v>222.22222222222223</v>
       </c>
-      <c r="K8" s="50">
+      <c r="K8" s="47">
         <v>7.5</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <v>10</v>
       </c>
-      <c r="M8" s="26">
-        <v>0.9</v>
-      </c>
-      <c r="N8" s="25">
+      <c r="M8" s="59">
+        <v>0.95</v>
+      </c>
+      <c r="N8" s="23">
         <v>5</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="24">
         <v>3</v>
       </c>
-      <c r="P8" s="27">
+      <c r="P8" s="25">
         <v>2.25</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="17">
         <f t="shared" si="4"/>
         <v>11.75</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="63">
         <f t="shared" si="5"/>
         <v>176.25</v>
       </c>
-      <c r="S8" s="55">
+      <c r="S8" s="50">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="41" t="s">
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="15">
-        <v>90</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="C9" s="60">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="H9" s="42">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I9" s="14">
         <v>4</v>
       </c>
-      <c r="F9" s="15">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="G9" s="8">
-        <f t="shared" si="1"/>
-        <v>360</v>
-      </c>
-      <c r="H9" s="44">
-        <f t="shared" si="2"/>
-        <v>1.1111111111111112</v>
-      </c>
-      <c r="I9" s="15">
-        <v>4</v>
-      </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <v>14</v>
       </c>
-      <c r="L9" s="45">
+      <c r="L9" s="43">
+        <v>3</v>
+      </c>
+      <c r="M9" s="58">
+        <v>0.85</v>
+      </c>
+      <c r="N9" s="41">
+        <v>3</v>
+      </c>
+      <c r="O9" s="42">
         <v>1</v>
       </c>
-      <c r="M9" s="44">
-        <v>0.85</v>
-      </c>
-      <c r="N9" s="43">
+      <c r="P9" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="Q9" s="16">
+        <f>N9*D9+O9*P9*D9</f>
+        <v>45</v>
+      </c>
+      <c r="R9" s="62">
+        <f t="shared" ref="R9" si="6">E9*Q9</f>
+        <v>112.5</v>
+      </c>
+      <c r="S9" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="60">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="2"/>
+        <v>360</v>
+      </c>
+      <c r="H10" s="42">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I10" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="K10" s="11">
+        <v>9</v>
+      </c>
+      <c r="L10" s="43">
+        <v>5</v>
+      </c>
+      <c r="M10" s="58">
+        <v>0.95</v>
+      </c>
+      <c r="N10" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="O10" s="42">
         <v>1</v>
       </c>
-      <c r="O9" s="44">
+      <c r="P10" s="48">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="16">
+        <f t="shared" ref="Q10:Q13" si="7">N10*D10+O10*P10*D10</f>
+        <v>13.5</v>
+      </c>
+      <c r="R10" s="62">
+        <f t="shared" ref="R10:R13" si="8">E10*Q10</f>
+        <v>54</v>
+      </c>
+      <c r="S10" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="60">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+      <c r="E11" s="14">
+        <v>1</v>
+      </c>
+      <c r="F11" s="65">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="H11" s="42">
+        <f t="shared" si="0"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="I11" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" si="3"/>
+        <v>10.989010989010989</v>
+      </c>
+      <c r="K11" s="68">
+        <v>21</v>
+      </c>
+      <c r="L11" s="67">
+        <v>2</v>
+      </c>
+      <c r="M11" s="66">
+        <v>0.4</v>
+      </c>
+      <c r="N11" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="Q11" s="16">
+        <f t="shared" si="7"/>
+        <v>30.9</v>
+      </c>
+      <c r="R11" s="62">
+        <f t="shared" si="8"/>
+        <v>30.9</v>
+      </c>
+      <c r="S11" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="60">
+        <v>140</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="H12" s="42">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="I12" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="J12" s="8">
+        <f t="shared" si="3"/>
+        <v>14.084507042253522</v>
+      </c>
+      <c r="K12" s="68">
+        <v>20</v>
+      </c>
+      <c r="L12" s="67">
+        <v>0</v>
+      </c>
+      <c r="M12" s="66">
+        <v>0.4</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5</v>
+      </c>
+      <c r="O12" s="1">
         <v>10</v>
       </c>
-      <c r="P9" s="52">
+      <c r="P12" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="Q12" s="16">
+        <f t="shared" si="7"/>
+        <v>22.5</v>
+      </c>
+      <c r="R12" s="62">
+        <f t="shared" si="8"/>
+        <v>22.5</v>
+      </c>
+      <c r="S12" s="1">
+        <v>90</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="60">
+        <v>75</v>
+      </c>
+      <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="Q9" s="17">
-        <f t="shared" ref="Q9" si="6">N9+O9*P9</f>
-        <v>11</v>
-      </c>
-      <c r="R9" s="17">
-        <f t="shared" ref="R9" si="7">E9*Q9</f>
-        <v>44</v>
-      </c>
-      <c r="S9" s="44">
-        <v>75</v>
+      <c r="E13" s="14">
+        <v>2</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="H13" s="42">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I13" s="14">
+        <v>5</v>
+      </c>
+      <c r="J13" s="8">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K13" s="11">
+        <v>10</v>
+      </c>
+      <c r="L13" s="43">
+        <v>0</v>
+      </c>
+      <c r="M13" s="58">
+        <v>0.7</v>
+      </c>
+      <c r="N13" s="42">
+        <v>4</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2</v>
+      </c>
+      <c r="P13" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="40">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="R13" s="62">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="S13" s="42">
+        <v>60</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="51"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G11" s="56"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S15" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Miniguns + Burst shooters + Weapon balance
</commit_message>
<xml_diff>
--- a/Other/weaponsBalance.xlsx
+++ b/Other/weaponsBalance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danit\Desktop\Github\Unity_MultiplayerGame\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8539F462-2901-4C8C-91CB-00B11ED424B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C387D8D-82E5-4343-BBF3-C03398F8AF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8BFD530-F1DB-4083-B445-48265BEB5EB8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="52">
   <si>
     <t>Wp</t>
   </si>
@@ -156,6 +156,42 @@
   </si>
   <si>
     <t>35-25</t>
+  </si>
+  <si>
+    <t>burst_short</t>
+  </si>
+  <si>
+    <t>burst_long</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Miniguns</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>70-50</t>
+  </si>
+  <si>
+    <t>indirect radius</t>
+  </si>
+  <si>
+    <t>main radius</t>
+  </si>
+  <si>
+    <t>Jump RNG</t>
+  </si>
+  <si>
+    <t>cost increase x bullet</t>
+  </si>
+  <si>
+    <t>recovery speed</t>
   </si>
 </sst>
 </file>
@@ -448,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -560,7 +596,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,7 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -632,9 +666,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -642,6 +673,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -958,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E3534C-2912-465D-8271-A50631F92518}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,17 +1050,22 @@
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" customWidth="1"/>
-    <col min="18" max="19" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="16" width="10.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
     <col min="20" max="20" width="12.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
@@ -1006,34 +1084,35 @@
       <c r="L2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="N2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="O2" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="Q2" s="15" t="s">
+      <c r="P2" s="3"/>
+      <c r="R2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="19" t="s">
+      <c r="S2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="51" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="28" t="s">
@@ -1060,39 +1139,54 @@
       <c r="L3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="54" t="s">
+      <c r="O3" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="55" t="s">
+      <c r="P3" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="56" t="s">
+      <c r="Q3" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="R3" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="33" t="s">
+      <c r="S3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="53" t="s">
+      <c r="T3" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="23" t="s">
         <v>36</v>
       </c>
+      <c r="V3" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" s="71" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="60">
+      <c r="C4" s="58">
         <v>36</v>
       </c>
       <c r="D4" s="1">
@@ -1110,7 +1204,7 @@
         <v>288</v>
       </c>
       <c r="H4" s="15">
-        <f t="shared" ref="H4:H13" si="0">100/C4</f>
+        <f t="shared" ref="H4:H10" si="0">100/C4</f>
         <v>2.7777777777777777</v>
       </c>
       <c r="I4" s="2">
@@ -1120,41 +1214,59 @@
         <f>100/I4</f>
         <v>125</v>
       </c>
-      <c r="K4" s="44">
+      <c r="K4" s="43">
         <v>15</v>
       </c>
-      <c r="L4" s="45">
+      <c r="L4" s="44">
         <v>3</v>
       </c>
-      <c r="M4" s="57">
+      <c r="M4" s="1">
+        <v>6</v>
+      </c>
+      <c r="N4" s="55">
         <v>0.75</v>
       </c>
-      <c r="N4" s="18">
+      <c r="O4" s="18">
         <v>3</v>
       </c>
-      <c r="O4" s="21">
+      <c r="P4" s="21">
         <v>3</v>
       </c>
-      <c r="P4" s="19">
+      <c r="Q4" s="19">
         <v>2</v>
       </c>
-      <c r="Q4" s="16">
-        <f>N4*D4+O4*P4*D4</f>
+      <c r="R4" s="16">
+        <f>O4*D4+P4*Q4*D4</f>
         <v>9</v>
       </c>
-      <c r="R4" s="62">
-        <f>E4*Q4</f>
+      <c r="S4" s="60">
+        <f>E4*R4</f>
         <v>72</v>
       </c>
-      <c r="S4" s="49">
+      <c r="T4" s="48">
         <v>50</v>
       </c>
+      <c r="U4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="58">
         <v>28</v>
       </c>
       <c r="D5" s="1">
@@ -1164,11 +1276,11 @@
         <v>10.3</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F13" si="1">1/E5</f>
+        <f t="shared" ref="F5:F10" si="1">1/E5</f>
         <v>9.7087378640776698E-2</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G13" si="2">C5*E5*D5</f>
+        <f t="shared" ref="G5:G10" si="2">C5*E5*D5</f>
         <v>288.40000000000003</v>
       </c>
       <c r="H5" s="16">
@@ -1179,44 +1291,62 @@
         <v>0.71</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" ref="J5:J13" si="3">100/I5</f>
+        <f t="shared" ref="J5:J10" si="3">100/I5</f>
         <v>140.84507042253523</v>
       </c>
-      <c r="K5" s="46">
+      <c r="K5" s="45">
         <v>15</v>
       </c>
       <c r="L5" s="12">
         <v>2.5</v>
       </c>
-      <c r="M5" s="58">
+      <c r="M5" s="1">
+        <v>6</v>
+      </c>
+      <c r="N5" s="56">
         <v>0.8</v>
       </c>
-      <c r="N5" s="20">
+      <c r="O5" s="20">
         <v>3</v>
       </c>
-      <c r="O5" s="21">
+      <c r="P5" s="21">
         <v>4</v>
       </c>
-      <c r="P5" s="22">
+      <c r="Q5" s="22">
         <v>2</v>
       </c>
-      <c r="Q5" s="16">
-        <f t="shared" ref="Q5:Q8" si="4">N5*D5+O5*P5*D5</f>
+      <c r="R5" s="16">
+        <f>O5*D5+P5*Q5*D5</f>
         <v>11</v>
       </c>
-      <c r="R5" s="62">
-        <f t="shared" ref="R5:R8" si="5">E5*Q5</f>
+      <c r="S5" s="60">
+        <f>E5*R5</f>
         <v>113.30000000000001</v>
       </c>
-      <c r="S5" s="40">
+      <c r="T5" s="39">
         <v>60</v>
       </c>
+      <c r="U5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="58">
         <v>52</v>
       </c>
       <c r="D6" s="1">
@@ -1244,41 +1374,59 @@
         <f t="shared" si="3"/>
         <v>60.606060606060609</v>
       </c>
-      <c r="K6" s="46">
+      <c r="K6" s="45">
         <v>18</v>
       </c>
       <c r="L6" s="12">
         <v>4.5</v>
       </c>
-      <c r="M6" s="58">
+      <c r="M6" s="1">
+        <v>7</v>
+      </c>
+      <c r="N6" s="56">
         <v>0.5</v>
       </c>
-      <c r="N6" s="20">
+      <c r="O6" s="20">
         <v>3.5</v>
       </c>
-      <c r="O6" s="21">
+      <c r="P6" s="21">
         <v>2</v>
       </c>
-      <c r="P6" s="22">
+      <c r="Q6" s="22">
         <v>2.25</v>
       </c>
-      <c r="Q6" s="16">
-        <f t="shared" si="4"/>
+      <c r="R6" s="16">
+        <f>O6*D6+P6*Q6*D6</f>
         <v>8</v>
       </c>
-      <c r="R6" s="62">
-        <f t="shared" si="5"/>
+      <c r="S6" s="60">
+        <f>E6*R6</f>
         <v>48</v>
       </c>
-      <c r="S6" s="40">
+      <c r="T6" s="39">
         <v>55</v>
       </c>
+      <c r="U6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X6" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="60">
+      <c r="C7" s="58">
         <v>42</v>
       </c>
       <c r="D7" s="1">
@@ -1306,41 +1454,59 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="K7" s="46">
+      <c r="K7" s="45">
         <v>28</v>
       </c>
       <c r="L7" s="12">
         <v>1.5</v>
       </c>
-      <c r="M7" s="58">
+      <c r="M7" s="1">
+        <v>3</v>
+      </c>
+      <c r="N7" s="56">
         <v>0.65</v>
       </c>
-      <c r="N7" s="20">
+      <c r="O7" s="20">
         <v>3.4</v>
       </c>
-      <c r="O7" s="21">
+      <c r="P7" s="21">
         <v>3</v>
       </c>
-      <c r="P7" s="22">
+      <c r="Q7" s="22">
         <v>2</v>
       </c>
-      <c r="Q7" s="16">
-        <f t="shared" si="4"/>
+      <c r="R7" s="16">
+        <f>O7*D7+P7*Q7*D7</f>
         <v>9.4</v>
       </c>
-      <c r="R7" s="62">
-        <f t="shared" si="5"/>
+      <c r="S7" s="60">
+        <f>E7*R7</f>
         <v>65.8</v>
       </c>
-      <c r="S7" s="40">
+      <c r="T7" s="39">
         <v>75</v>
       </c>
+      <c r="U7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="59">
         <v>33</v>
       </c>
       <c r="D8" s="24">
@@ -1353,7 +1519,7 @@
         <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="50">
         <f t="shared" si="2"/>
         <v>495</v>
       </c>
@@ -1369,363 +1535,982 @@
         <f t="shared" si="3"/>
         <v>222.22222222222223</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="46">
         <v>7.5</v>
       </c>
       <c r="L8" s="13">
         <v>10</v>
       </c>
-      <c r="M8" s="59">
+      <c r="M8" s="24">
+        <v>20</v>
+      </c>
+      <c r="N8" s="57">
         <v>0.95</v>
       </c>
-      <c r="N8" s="23">
+      <c r="O8" s="23">
         <v>5</v>
       </c>
-      <c r="O8" s="24">
+      <c r="P8" s="24">
         <v>3</v>
       </c>
-      <c r="P8" s="25">
+      <c r="Q8" s="25">
         <v>2.25</v>
       </c>
-      <c r="Q8" s="17">
-        <f t="shared" si="4"/>
+      <c r="R8" s="17">
+        <f>O8*D8+P8*Q8*D8</f>
         <v>11.75</v>
       </c>
-      <c r="R8" s="63">
-        <f t="shared" si="5"/>
+      <c r="S8" s="61">
+        <f>E8*R8</f>
         <v>176.25</v>
       </c>
-      <c r="S8" s="50">
+      <c r="T8" s="49">
         <v>50</v>
       </c>
+      <c r="U8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="V8" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="W8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" s="67" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="60">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1">
-        <v>10</v>
+    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="58">
+        <v>30</v>
+      </c>
+      <c r="D9" s="41">
+        <v>3</v>
       </c>
       <c r="E9" s="14">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F9" s="14">
         <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="G9" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G9" s="66">
         <f t="shared" si="2"/>
-        <v>250</v>
-      </c>
-      <c r="H9" s="42">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I9" s="14">
-        <v>4</v>
-      </c>
-      <c r="J9" s="8">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="K9" s="11">
-        <v>14</v>
-      </c>
-      <c r="L9" s="43">
-        <v>3</v>
-      </c>
-      <c r="M9" s="58">
-        <v>0.85</v>
-      </c>
-      <c r="N9" s="41">
-        <v>3</v>
-      </c>
-      <c r="O9" s="42">
-        <v>1</v>
-      </c>
-      <c r="P9" s="48">
-        <v>1.5</v>
-      </c>
-      <c r="Q9" s="16">
-        <f>N9*D9+O9*P9*D9</f>
-        <v>45</v>
-      </c>
-      <c r="R9" s="62">
-        <f t="shared" ref="R9" si="6">E9*Q9</f>
-        <v>112.5</v>
-      </c>
-      <c r="S9" s="42">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="60">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3</v>
-      </c>
-      <c r="E10" s="14">
-        <v>4</v>
-      </c>
-      <c r="F10" s="14">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" si="2"/>
-        <v>360</v>
-      </c>
-      <c r="H10" s="42">
+        <v>270</v>
+      </c>
+      <c r="H9" s="39">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I9" s="14">
+        <v>1.95</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="3"/>
+        <v>51.282051282051285</v>
+      </c>
+      <c r="K9" s="45">
+        <v>15</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="56">
+        <v>0.7</v>
+      </c>
+      <c r="O9" s="40">
+        <v>3</v>
+      </c>
+      <c r="P9" s="41">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="47">
+        <v>2</v>
+      </c>
+      <c r="R9" s="17">
+        <f>O9*D9+P9*Q9*D9</f>
+        <v>27</v>
+      </c>
+      <c r="S9" s="61">
+        <f>E9*R9</f>
+        <v>81</v>
+      </c>
+      <c r="T9" s="39">
+        <v>60</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="59">
+        <v>30</v>
+      </c>
+      <c r="D10" s="71">
+        <v>4</v>
+      </c>
+      <c r="E10" s="72">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="72">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G10" s="50">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="H10" s="49">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I10" s="72">
+        <v>2.25</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="3"/>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="K10" s="46">
+        <v>22</v>
+      </c>
+      <c r="L10" s="73">
+        <v>0</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0</v>
+      </c>
+      <c r="N10" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="O10" s="74">
+        <v>3</v>
+      </c>
+      <c r="P10" s="71">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="75">
+        <v>2</v>
+      </c>
+      <c r="R10" s="17">
+        <f>O10*D10+P10*Q10*D10</f>
+        <v>44</v>
+      </c>
+      <c r="S10" s="61">
+        <f>E10*R10</f>
+        <v>66</v>
+      </c>
+      <c r="T10" s="74">
+        <v>60</v>
+      </c>
+      <c r="U10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="V10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="W10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="X10" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="58">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10</v>
+      </c>
+      <c r="E11" s="14">
+        <v>2</v>
+      </c>
+      <c r="F11" s="14">
+        <f>1/E11</f>
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="7">
+        <f>C11*E11*D11</f>
+        <v>200</v>
+      </c>
+      <c r="H11" s="41">
+        <f>100/C11</f>
+        <v>10</v>
+      </c>
+      <c r="I11" s="14">
+        <v>4</v>
+      </c>
+      <c r="J11" s="8">
+        <f>100/I11</f>
+        <v>25</v>
+      </c>
+      <c r="K11" s="11">
+        <v>14</v>
+      </c>
+      <c r="L11" s="42">
+        <v>3</v>
+      </c>
+      <c r="M11" s="1">
+        <v>3</v>
+      </c>
+      <c r="N11" s="56">
+        <v>0.85</v>
+      </c>
+      <c r="O11" s="40">
+        <v>3</v>
+      </c>
+      <c r="P11" s="41">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="R11" s="16">
+        <f>O11*D11+P11*Q11*D11</f>
+        <v>45</v>
+      </c>
+      <c r="S11" s="60">
+        <f>E11*R11</f>
+        <v>90</v>
+      </c>
+      <c r="T11" s="41">
+        <v>75</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X11" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="58">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="14">
+        <v>4</v>
+      </c>
+      <c r="F12" s="14">
+        <f>1/E12</f>
+        <v>0.25</v>
+      </c>
+      <c r="G12" s="7">
+        <f>C12*E12*D12</f>
+        <v>300</v>
+      </c>
+      <c r="H12" s="41">
+        <f>100/C12</f>
+        <v>4</v>
+      </c>
+      <c r="I12" s="14">
         <v>2.5</v>
       </c>
-      <c r="J10" s="8">
-        <f t="shared" si="3"/>
+      <c r="J12" s="8">
+        <f>100/I12</f>
         <v>40</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K12" s="11">
         <v>9</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L12" s="42">
         <v>5</v>
       </c>
-      <c r="M10" s="58">
+      <c r="M12" s="1">
+        <v>5</v>
+      </c>
+      <c r="N12" s="56">
         <v>0.95</v>
       </c>
-      <c r="N10" s="41">
+      <c r="O12" s="40">
         <v>2.5</v>
       </c>
-      <c r="O10" s="42">
+      <c r="P12" s="41">
         <v>1</v>
       </c>
-      <c r="P10" s="48">
+      <c r="Q12" s="47">
         <v>2</v>
       </c>
-      <c r="Q10" s="16">
-        <f t="shared" ref="Q10:Q13" si="7">N10*D10+O10*P10*D10</f>
+      <c r="R12" s="16">
+        <f>O12*D12+P12*Q12*D12</f>
         <v>13.5</v>
       </c>
-      <c r="R10" s="62">
-        <f t="shared" ref="R10:R13" si="8">E10*Q10</f>
+      <c r="S12" s="60">
+        <f>E12*R12</f>
         <v>54</v>
       </c>
-      <c r="S10" s="42">
+      <c r="T12" s="41">
         <v>75</v>
       </c>
+      <c r="U12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="60">
+      <c r="C13" s="59">
         <v>35</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D13" s="24">
         <v>6</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E13" s="72">
         <v>1</v>
       </c>
-      <c r="F11" s="65">
-        <f t="shared" si="1"/>
+      <c r="F13" s="77">
+        <f>1/E13</f>
         <v>1</v>
       </c>
-      <c r="G11" s="7">
-        <f t="shared" si="2"/>
+      <c r="G13" s="78">
+        <f>C13*E13*D13</f>
         <v>210</v>
       </c>
-      <c r="H11" s="42">
-        <f t="shared" si="0"/>
+      <c r="H13" s="71">
+        <f>100/C13</f>
         <v>2.8571428571428572</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I13" s="24">
         <v>9.1</v>
       </c>
-      <c r="J11" s="8">
-        <f t="shared" si="3"/>
+      <c r="J13" s="9">
+        <f>100/I13</f>
         <v>10.989010989010989</v>
       </c>
-      <c r="K11" s="68">
+      <c r="K13" s="79">
         <v>21</v>
       </c>
-      <c r="L11" s="67">
+      <c r="L13" s="73">
         <v>2</v>
       </c>
-      <c r="M11" s="66">
+      <c r="M13" s="24">
+        <v>2</v>
+      </c>
+      <c r="N13" s="57">
         <v>0.4</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O13" s="24">
         <v>3.4</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P13" s="24">
         <v>1</v>
       </c>
-      <c r="P11" s="1">
+      <c r="Q13" s="24">
         <v>1.75</v>
       </c>
-      <c r="Q11" s="16">
-        <f t="shared" si="7"/>
+      <c r="R13" s="17">
+        <f>O13*D13+P13*Q13*D13</f>
         <v>30.9</v>
       </c>
-      <c r="R11" s="62">
-        <f t="shared" si="8"/>
+      <c r="S13" s="61">
+        <f>E13*R13</f>
         <v>30.9</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T13" s="24">
         <v>75</v>
       </c>
+      <c r="U13" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="V13" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="W13" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="X13" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B14" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="60">
+      <c r="C14" s="58">
         <v>140</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="1"/>
+      <c r="F14" s="1">
+        <f>1/E14</f>
         <v>1</v>
       </c>
-      <c r="G12" s="7">
-        <f t="shared" si="2"/>
+      <c r="G14" s="7">
+        <f>C14*E14*D14</f>
         <v>140</v>
       </c>
-      <c r="H12" s="42">
-        <f t="shared" si="0"/>
+      <c r="H14" s="41">
+        <f>100/C14</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="I12" s="1">
-        <v>7.1</v>
-      </c>
-      <c r="J12" s="8">
-        <f t="shared" si="3"/>
-        <v>14.084507042253522</v>
-      </c>
-      <c r="K12" s="68">
+      <c r="I14" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="J14" s="8">
+        <f>100/I14</f>
+        <v>11.764705882352942</v>
+      </c>
+      <c r="K14" s="65">
         <v>20</v>
       </c>
-      <c r="L12" s="67">
+      <c r="L14" s="64">
         <v>0</v>
       </c>
-      <c r="M12" s="66">
+      <c r="M14" s="1">
+        <v>2</v>
+      </c>
+      <c r="N14" s="63">
         <v>0.4</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O14" s="1">
         <v>5</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P14" s="1">
         <v>10</v>
       </c>
-      <c r="P12" s="1">
+      <c r="Q14" s="1">
         <v>1.75</v>
       </c>
-      <c r="Q12" s="16">
-        <f t="shared" si="7"/>
+      <c r="R14" s="16">
+        <f>O14*D14+P14*Q14*D14</f>
         <v>22.5</v>
       </c>
-      <c r="R12" s="62">
-        <f t="shared" si="8"/>
+      <c r="S14" s="60">
+        <f>E14*R14</f>
         <v>22.5</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T14" s="1">
         <v>90</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="V14" s="1">
+        <v>2</v>
+      </c>
+      <c r="W14" s="1">
+        <v>4</v>
+      </c>
+      <c r="X14" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="64" t="s">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="60">
+      <c r="C15" s="58">
+        <v>85</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14">
+        <v>2</v>
+      </c>
+      <c r="F15" s="14">
+        <f>1/E15</f>
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="7">
+        <f>C15*E15*D15</f>
+        <v>170</v>
+      </c>
+      <c r="H15" s="41">
+        <f>100/C15</f>
+        <v>1.1764705882352942</v>
+      </c>
+      <c r="I15" s="14">
+        <v>5</v>
+      </c>
+      <c r="J15" s="8">
+        <f>100/I15</f>
+        <v>20</v>
+      </c>
+      <c r="K15" s="11">
+        <v>13</v>
+      </c>
+      <c r="L15" s="42">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15" s="56">
+        <v>0.7</v>
+      </c>
+      <c r="O15" s="41">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>2</v>
+      </c>
+      <c r="R15" s="39">
+        <f>O15*D15+P15*Q15*D15</f>
+        <v>14</v>
+      </c>
+      <c r="S15" s="60">
+        <f>E15*R15</f>
+        <v>28</v>
+      </c>
+      <c r="T15" s="41">
         <v>75</v>
       </c>
-      <c r="D13" s="1">
+      <c r="U15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V15" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="14">
+      <c r="W15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="X15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="59">
+        <v>140</v>
+      </c>
+      <c r="D16" s="24">
+        <v>1</v>
+      </c>
+      <c r="E16" s="72">
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="72">
+        <f>1/E16</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G16" s="78">
+        <f>C16*E16*D16</f>
+        <v>210</v>
+      </c>
+      <c r="H16" s="71">
+        <f>100/C16</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="I16" s="24">
+        <v>6</v>
+      </c>
+      <c r="J16" s="24">
+        <f>100/I16</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="K16" s="24">
+        <v>8</v>
+      </c>
+      <c r="L16" s="24">
+        <v>0</v>
+      </c>
+      <c r="M16" s="24">
         <v>2</v>
       </c>
-      <c r="F13" s="14">
-        <f t="shared" si="1"/>
+      <c r="N16" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="O16" s="24">
+        <v>4.5</v>
+      </c>
+      <c r="P16" s="24">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="24">
+        <v>2</v>
+      </c>
+      <c r="R16" s="24">
+        <f>O16*D16+P16*Q16*D16</f>
+        <v>8.5</v>
+      </c>
+      <c r="S16" s="24">
+        <f>E16*R16</f>
+        <v>12.75</v>
+      </c>
+      <c r="T16" s="24">
+        <v>70</v>
+      </c>
+      <c r="U16" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="V16" s="24">
+        <v>2</v>
+      </c>
+      <c r="W16" s="24">
+        <v>4.25</v>
+      </c>
+      <c r="X16" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="58">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1">
+        <f>1/E17</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <f>C17*E17*D17</f>
+        <v>416</v>
+      </c>
+      <c r="H17" s="41">
+        <f>100/C17</f>
+        <v>3.125</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="1">
+        <f>100/I17</f>
+        <v>1000</v>
+      </c>
+      <c r="K17" s="1">
+        <v>24</v>
+      </c>
+      <c r="L17" s="1">
+        <v>7</v>
+      </c>
+      <c r="M17" s="1">
+        <v>14</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O17" s="1">
+        <v>3</v>
+      </c>
+      <c r="P17" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>2</v>
+      </c>
+      <c r="R17" s="1">
+        <f>O17*D17+P17*Q17*D17</f>
+        <v>7</v>
+      </c>
+      <c r="S17" s="1">
+        <f>E17*R17</f>
+        <v>91</v>
+      </c>
+      <c r="T17" s="1">
+        <v>50</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X17" s="41">
+        <v>0.02</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="58">
+        <v>29</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" ref="F18:F19" si="4">1/E18</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <f>C18*E18*D18</f>
+        <v>522</v>
+      </c>
+      <c r="H18" s="41">
+        <f>100/C18</f>
+        <v>3.4482758620689653</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="1">
+        <f>100/I18</f>
+        <v>1000</v>
+      </c>
+      <c r="K18" s="1">
+        <v>18</v>
+      </c>
+      <c r="L18" s="1">
+        <v>8</v>
+      </c>
+      <c r="M18" s="1">
+        <v>16</v>
+      </c>
+      <c r="N18" s="1">
         <v>0.5</v>
       </c>
-      <c r="G13" s="7">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-      <c r="H13" s="42">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="I13" s="14">
+      <c r="O18" s="1">
+        <v>3</v>
+      </c>
+      <c r="P18" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>2</v>
+      </c>
+      <c r="R18" s="1">
+        <f>O18*D18+P18*Q18*D18</f>
+        <v>7</v>
+      </c>
+      <c r="S18" s="1">
+        <f>E18*R18</f>
+        <v>126</v>
+      </c>
+      <c r="T18" s="1">
+        <v>50</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X18" s="41">
+        <v>0.01</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="58">
+        <v>41</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="4"/>
+        <v>0.04</v>
+      </c>
+      <c r="G19" s="1">
+        <f>C19*E19*D19</f>
+        <v>1025</v>
+      </c>
+      <c r="H19" s="41">
+        <f>100/C19</f>
+        <v>2.4390243902439024</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="1">
+        <f>100/I19</f>
+        <v>1000</v>
+      </c>
+      <c r="K19" s="1">
+        <v>30</v>
+      </c>
+      <c r="L19" s="1">
+        <v>6</v>
+      </c>
+      <c r="M19" s="1">
+        <v>12</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>3</v>
+      </c>
+      <c r="P19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>2</v>
+      </c>
+      <c r="R19" s="1">
+        <f>O19*D19+P19*Q19*D19</f>
         <v>5</v>
       </c>
-      <c r="J13" s="8">
-        <f t="shared" si="3"/>
+      <c r="S19" s="1">
+        <f>E19*R19</f>
+        <v>125</v>
+      </c>
+      <c r="T19" s="1">
+        <v>75</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X19" s="41">
+        <v>2.3E-2</v>
+      </c>
+      <c r="Y19" s="1">
         <v>20</v>
       </c>
-      <c r="K13" s="11">
-        <v>10</v>
-      </c>
-      <c r="L13" s="43">
-        <v>0</v>
-      </c>
-      <c r="M13" s="58">
-        <v>0.7</v>
-      </c>
-      <c r="N13" s="42">
-        <v>4</v>
-      </c>
-      <c r="O13" s="1">
-        <v>2</v>
-      </c>
-      <c r="P13" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="40">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="R13" s="62">
-        <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-      <c r="S13" s="42">
-        <v>60</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="51"/>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="Y20" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="S15" s="51"/>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y25" s="1"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Weapons Adjustments + 60fps cap
+ 60 fps Cap
+ Same Version needed for Net

+ All Weapons Range Reduction
+ Remade Blasters DMG
+ Linear Paint Droplets (For Blasters)
</commit_message>
<xml_diff>
--- a/Other/weaponsBalance.xlsx
+++ b/Other/weaponsBalance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danit\Desktop\Github\Unity_MultiplayerGame\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C387D8D-82E5-4343-BBF3-C03398F8AF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443E792D-509E-498E-8F44-7386C072D5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8BFD530-F1DB-4083-B445-48265BEB5EB8}"/>
   </bookViews>
@@ -1034,7 +1034,7 @@
   <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,15 +1193,15 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2">
         <f>1/E4</f>
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="G4" s="7">
         <f>C4*E4*D4</f>
-        <v>288</v>
+        <v>360</v>
       </c>
       <c r="H4" s="15">
         <f t="shared" ref="H4:H10" si="0">100/C4</f>
@@ -1215,7 +1215,7 @@
         <v>125</v>
       </c>
       <c r="K4" s="43">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L4" s="44">
         <v>3</v>
@@ -1230,18 +1230,18 @@
         <v>3</v>
       </c>
       <c r="P4" s="21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="19">
         <v>2</v>
       </c>
       <c r="R4" s="16">
-        <f>O4*D4+P4*Q4*D4</f>
-        <v>9</v>
+        <f t="shared" ref="R4:R19" si="1">O4*D4+P4*Q4*D4</f>
+        <v>5</v>
       </c>
       <c r="S4" s="60">
-        <f>E4*R4</f>
-        <v>72</v>
+        <f t="shared" ref="S4:S19" si="2">E4*R4</f>
+        <v>50</v>
       </c>
       <c r="T4" s="48">
         <v>50</v>
@@ -1273,15 +1273,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>10.3</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F10" si="1">1/E5</f>
-        <v>9.7087378640776698E-2</v>
+        <f t="shared" ref="F5:F10" si="3">1/E5</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G10" si="2">C5*E5*D5</f>
-        <v>288.40000000000003</v>
+        <f t="shared" ref="G5:G10" si="4">C5*E5*D5</f>
+        <v>336</v>
       </c>
       <c r="H5" s="16">
         <f t="shared" si="0"/>
@@ -1291,11 +1291,11 @@
         <v>0.71</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" ref="J5:J10" si="3">100/I5</f>
+        <f t="shared" ref="J5:J10" si="5">100/I5</f>
         <v>140.84507042253523</v>
       </c>
       <c r="K5" s="45">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L5" s="12">
         <v>2.5</v>
@@ -1310,18 +1310,18 @@
         <v>3</v>
       </c>
       <c r="P5" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="22">
         <v>2</v>
       </c>
       <c r="R5" s="16">
-        <f>O5*D5+P5*Q5*D5</f>
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="S5" s="60">
-        <f>E5*R5</f>
-        <v>113.30000000000001</v>
+        <f t="shared" si="2"/>
+        <v>60</v>
       </c>
       <c r="T5" s="39">
         <v>60</v>
@@ -1353,15 +1353,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>6</v>
+        <v>6.67</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <f t="shared" si="3"/>
+        <v>0.14992503748125938</v>
       </c>
       <c r="G6" s="7">
-        <f t="shared" si="2"/>
-        <v>312</v>
+        <f t="shared" si="4"/>
+        <v>346.84</v>
       </c>
       <c r="H6" s="16">
         <f t="shared" si="0"/>
@@ -1371,11 +1371,11 @@
         <v>1.65</v>
       </c>
       <c r="J6" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>60.606060606060609</v>
       </c>
       <c r="K6" s="45">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="L6" s="12">
         <v>4.5</v>
@@ -1390,18 +1390,18 @@
         <v>3.5</v>
       </c>
       <c r="P6" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="22">
         <v>2.25</v>
       </c>
       <c r="R6" s="16">
-        <f>O6*D6+P6*Q6*D6</f>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>5.75</v>
       </c>
       <c r="S6" s="60">
-        <f>E6*R6</f>
-        <v>48</v>
+        <f t="shared" si="2"/>
+        <v>38.352499999999999</v>
       </c>
       <c r="T6" s="39">
         <v>55</v>
@@ -1433,15 +1433,15 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.14285714285714285</v>
+        <f t="shared" si="3"/>
+        <v>0.125</v>
       </c>
       <c r="G7" s="7">
-        <f t="shared" si="2"/>
-        <v>294</v>
+        <f t="shared" si="4"/>
+        <v>336</v>
       </c>
       <c r="H7" s="16">
         <f t="shared" si="0"/>
@@ -1451,11 +1451,11 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
       <c r="K7" s="45">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L7" s="12">
         <v>1.5</v>
@@ -1470,18 +1470,18 @@
         <v>3.4</v>
       </c>
       <c r="P7" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="22">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="R7" s="16">
-        <f>O7*D7+P7*Q7*D7</f>
-        <v>9.4</v>
+        <f t="shared" si="1"/>
+        <v>6.9</v>
       </c>
       <c r="S7" s="60">
-        <f>E7*R7</f>
-        <v>65.8</v>
+        <f t="shared" si="2"/>
+        <v>55.2</v>
       </c>
       <c r="T7" s="39">
         <v>75</v>
@@ -1507,36 +1507,36 @@
         <v>7</v>
       </c>
       <c r="C8" s="59">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D8" s="24">
         <v>1</v>
       </c>
       <c r="E8" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="1"/>
-        <v>6.6666666666666666E-2</v>
+        <f t="shared" si="3"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G8" s="50">
-        <f t="shared" si="2"/>
-        <v>495</v>
+        <f t="shared" si="4"/>
+        <v>456</v>
       </c>
       <c r="H8" s="17">
         <f t="shared" si="0"/>
-        <v>3.0303030303030303</v>
+        <v>2.6315789473684212</v>
       </c>
       <c r="I8" s="4">
         <f>0.45</f>
         <v>0.45</v>
       </c>
       <c r="J8" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>222.22222222222223</v>
       </c>
       <c r="K8" s="46">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="L8" s="13">
         <v>10</v>
@@ -1548,21 +1548,21 @@
         <v>0.95</v>
       </c>
       <c r="O8" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P8" s="24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="25">
         <v>2.25</v>
       </c>
       <c r="R8" s="17">
-        <f>O8*D8+P8*Q8*D8</f>
-        <v>11.75</v>
+        <f t="shared" si="1"/>
+        <v>6.25</v>
       </c>
       <c r="S8" s="61">
-        <f>E8*R8</f>
-        <v>176.25</v>
+        <f t="shared" si="2"/>
+        <v>75</v>
       </c>
       <c r="T8" s="49">
         <v>50</v>
@@ -1597,11 +1597,11 @@
         <v>3</v>
       </c>
       <c r="F9" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G9" s="66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>270</v>
       </c>
       <c r="H9" s="39">
@@ -1612,11 +1612,11 @@
         <v>1.95</v>
       </c>
       <c r="J9" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>51.282051282051285</v>
       </c>
       <c r="K9" s="45">
-        <v>15</v>
+        <v>13.5</v>
       </c>
       <c r="L9" s="12">
         <v>0</v>
@@ -1637,11 +1637,11 @@
         <v>2</v>
       </c>
       <c r="R9" s="17">
-        <f>O9*D9+P9*Q9*D9</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="S9" s="61">
-        <f>E9*R9</f>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="T9" s="39">
@@ -1677,11 +1677,11 @@
         <v>1.5</v>
       </c>
       <c r="F10" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="G10" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="H10" s="49">
@@ -1692,11 +1692,11 @@
         <v>2.25</v>
       </c>
       <c r="J10" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44.444444444444443</v>
       </c>
       <c r="K10" s="46">
-        <v>22</v>
+        <v>16.5</v>
       </c>
       <c r="L10" s="73">
         <v>0</v>
@@ -1717,11 +1717,11 @@
         <v>2</v>
       </c>
       <c r="R10" s="17">
-        <f>O10*D10+P10*Q10*D10</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="S10" s="61">
-        <f>E10*R10</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="T10" s="74">
@@ -1751,35 +1751,35 @@
         <v>4</v>
       </c>
       <c r="C11" s="58">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" s="14">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="F11" s="14">
         <f>1/E11</f>
-        <v>0.5</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G11" s="7">
-        <f>C11*E11*D11</f>
-        <v>200</v>
+        <f t="shared" ref="G11:G19" si="6">C11*E11*D11</f>
+        <v>204.75</v>
       </c>
       <c r="H11" s="41">
-        <f>100/C11</f>
-        <v>10</v>
+        <f t="shared" ref="H11:H19" si="7">100/C11</f>
+        <v>7.6923076923076925</v>
       </c>
       <c r="I11" s="14">
         <v>4</v>
       </c>
       <c r="J11" s="8">
-        <f>100/I11</f>
+        <f t="shared" ref="J11:J19" si="8">100/I11</f>
         <v>25</v>
       </c>
       <c r="K11" s="11">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L11" s="42">
         <v>3</v>
@@ -1800,12 +1800,12 @@
         <v>1.5</v>
       </c>
       <c r="R11" s="16">
-        <f>O11*D11+P11*Q11*D11</f>
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>31.5</v>
       </c>
       <c r="S11" s="60">
-        <f>E11*R11</f>
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>70.875</v>
       </c>
       <c r="T11" s="41">
         <v>75</v>
@@ -1837,29 +1837,29 @@
         <v>3</v>
       </c>
       <c r="E12" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="14">
-        <f>1/E12</f>
-        <v>0.25</v>
+        <f t="shared" ref="F11:F17" si="9">1/E12</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G12" s="7">
-        <f>C12*E12*D12</f>
-        <v>300</v>
+        <f t="shared" si="6"/>
+        <v>225</v>
       </c>
       <c r="H12" s="41">
-        <f>100/C12</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I12" s="14">
         <v>2.5</v>
       </c>
       <c r="J12" s="8">
-        <f>100/I12</f>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="K12" s="11">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="L12" s="42">
         <v>5</v>
@@ -1877,15 +1877,15 @@
         <v>1</v>
       </c>
       <c r="Q12" s="47">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="R12" s="16">
-        <f>O12*D12+P12*Q12*D12</f>
-        <v>13.5</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="S12" s="60">
-        <f>E12*R12</f>
-        <v>54</v>
+        <f t="shared" si="2"/>
+        <v>45</v>
       </c>
       <c r="T12" s="41">
         <v>75</v>
@@ -1920,26 +1920,26 @@
         <v>1</v>
       </c>
       <c r="F13" s="77">
-        <f>1/E13</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="G13" s="78">
-        <f>C13*E13*D13</f>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
       <c r="H13" s="71">
-        <f>100/C13</f>
+        <f t="shared" si="7"/>
         <v>2.8571428571428572</v>
       </c>
       <c r="I13" s="24">
         <v>9.1</v>
       </c>
       <c r="J13" s="9">
-        <f>100/I13</f>
+        <f t="shared" si="8"/>
         <v>10.989010989010989</v>
       </c>
       <c r="K13" s="79">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L13" s="73">
         <v>2</v>
@@ -1960,11 +1960,11 @@
         <v>1.75</v>
       </c>
       <c r="R13" s="17">
-        <f>O13*D13+P13*Q13*D13</f>
+        <f t="shared" si="1"/>
         <v>30.9</v>
       </c>
       <c r="S13" s="61">
-        <f>E13*R13</f>
+        <f t="shared" si="2"/>
         <v>30.9</v>
       </c>
       <c r="T13" s="24">
@@ -2003,26 +2003,26 @@
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <f>1/E14</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="G14" s="7">
-        <f>C14*E14*D14</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="H14" s="41">
-        <f>100/C14</f>
+        <f t="shared" si="7"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="I14" s="1">
         <v>8.5</v>
       </c>
       <c r="J14" s="8">
-        <f>100/I14</f>
+        <f t="shared" si="8"/>
         <v>11.764705882352942</v>
       </c>
       <c r="K14" s="65">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L14" s="64">
         <v>0</v>
@@ -2034,7 +2034,7 @@
         <v>0.4</v>
       </c>
       <c r="O14" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P14" s="1">
         <v>10</v>
@@ -2043,12 +2043,12 @@
         <v>1.75</v>
       </c>
       <c r="R14" s="16">
-        <f>O14*D14+P14*Q14*D14</f>
-        <v>22.5</v>
+        <f t="shared" si="1"/>
+        <v>21.5</v>
       </c>
       <c r="S14" s="60">
-        <f>E14*R14</f>
-        <v>22.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="T14" s="1">
         <v>90</v>
@@ -2083,26 +2083,26 @@
         <v>2</v>
       </c>
       <c r="F15" s="14">
-        <f>1/E15</f>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="G15" s="7">
-        <f>C15*E15*D15</f>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="H15" s="41">
-        <f>100/C15</f>
+        <f t="shared" si="7"/>
         <v>1.1764705882352942</v>
       </c>
       <c r="I15" s="14">
         <v>5</v>
       </c>
       <c r="J15" s="8">
-        <f>100/I15</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="K15" s="11">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L15" s="42">
         <v>0</v>
@@ -2114,7 +2114,7 @@
         <v>0.7</v>
       </c>
       <c r="O15" s="41">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="P15" s="1">
         <v>6</v>
@@ -2123,12 +2123,12 @@
         <v>2</v>
       </c>
       <c r="R15" s="39">
-        <f>O15*D15+P15*Q15*D15</f>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>14.5</v>
       </c>
       <c r="S15" s="60">
-        <f>E15*R15</f>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="T15" s="41">
         <v>75</v>
@@ -2163,22 +2163,22 @@
         <v>1.5</v>
       </c>
       <c r="F16" s="72">
-        <f>1/E16</f>
+        <f t="shared" si="9"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="G16" s="78">
-        <f>C16*E16*D16</f>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
       <c r="H16" s="71">
-        <f>100/C16</f>
+        <f t="shared" si="7"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="I16" s="24">
         <v>6</v>
       </c>
       <c r="J16" s="24">
-        <f>100/I16</f>
+        <f t="shared" si="8"/>
         <v>16.666666666666668</v>
       </c>
       <c r="K16" s="24">
@@ -2194,7 +2194,7 @@
         <v>0.75</v>
       </c>
       <c r="O16" s="24">
-        <v>4.5</v>
+        <v>4.25</v>
       </c>
       <c r="P16" s="24">
         <v>2</v>
@@ -2203,12 +2203,12 @@
         <v>2</v>
       </c>
       <c r="R16" s="24">
-        <f>O16*D16+P16*Q16*D16</f>
-        <v>8.5</v>
+        <f t="shared" si="1"/>
+        <v>8.25</v>
       </c>
       <c r="S16" s="24">
-        <f>E16*R16</f>
-        <v>12.75</v>
+        <f t="shared" si="2"/>
+        <v>12.375</v>
       </c>
       <c r="T16" s="24">
         <v>70</v>
@@ -2246,26 +2246,26 @@
         <v>13</v>
       </c>
       <c r="F17" s="1">
-        <f>1/E17</f>
+        <f t="shared" si="9"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="G17" s="1">
-        <f>C17*E17*D17</f>
+        <f t="shared" si="6"/>
         <v>416</v>
       </c>
       <c r="H17" s="41">
-        <f>100/C17</f>
+        <f t="shared" si="7"/>
         <v>3.125</v>
       </c>
       <c r="I17" s="1">
         <v>0.1</v>
       </c>
       <c r="J17" s="1">
-        <f>100/I17</f>
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
       <c r="K17" s="1">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="L17" s="1">
         <v>7</v>
@@ -2280,18 +2280,18 @@
         <v>3</v>
       </c>
       <c r="P17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="1">
         <v>2</v>
       </c>
       <c r="R17" s="1">
-        <f>O17*D17+P17*Q17*D17</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="S17" s="1">
-        <f>E17*R17</f>
-        <v>91</v>
+        <f t="shared" si="2"/>
+        <v>65</v>
       </c>
       <c r="T17" s="1">
         <v>50</v>
@@ -2326,26 +2326,26 @@
         <v>18</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" ref="F18:F19" si="4">1/E18</f>
+        <f t="shared" ref="F18:F19" si="10">1/E18</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="G18" s="1">
-        <f>C18*E18*D18</f>
+        <f t="shared" si="6"/>
         <v>522</v>
       </c>
       <c r="H18" s="41">
-        <f>100/C18</f>
+        <f t="shared" si="7"/>
         <v>3.4482758620689653</v>
       </c>
       <c r="I18" s="1">
         <v>0.1</v>
       </c>
       <c r="J18" s="1">
-        <f>100/I18</f>
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
       <c r="K18" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L18" s="1">
         <v>8</v>
@@ -2360,18 +2360,18 @@
         <v>3</v>
       </c>
       <c r="P18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="1">
         <v>2</v>
       </c>
       <c r="R18" s="1">
-        <f>O18*D18+P18*Q18*D18</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="S18" s="1">
-        <f>E18*R18</f>
-        <v>126</v>
+        <f t="shared" si="2"/>
+        <v>90</v>
       </c>
       <c r="T18" s="1">
         <v>50</v>
@@ -2406,26 +2406,26 @@
         <v>25</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0.04</v>
       </c>
       <c r="G19" s="1">
-        <f>C19*E19*D19</f>
+        <f t="shared" si="6"/>
         <v>1025</v>
       </c>
       <c r="H19" s="41">
-        <f>100/C19</f>
+        <f t="shared" si="7"/>
         <v>2.4390243902439024</v>
       </c>
       <c r="I19" s="1">
         <v>0.1</v>
       </c>
       <c r="J19" s="1">
-        <f>100/I19</f>
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
       <c r="K19" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L19" s="1">
         <v>6</v>
@@ -2446,11 +2446,11 @@
         <v>2</v>
       </c>
       <c r="R19" s="1">
-        <f>O19*D19+P19*Q19*D19</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="S19" s="1">
-        <f>E19*R19</f>
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
       <c r="T19" s="1">

</xml_diff>